<commit_message>
update giao diện tổng quan và chức năng
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6920" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6920"/>
   </bookViews>
   <sheets>
     <sheet name="Tiêu chuẩn TMĐT ĐG (CTN009)" sheetId="1" r:id="rId1"/>
@@ -1256,8 +1256,8 @@
   <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -1357,16 +1357,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <f>ROUNDUP(B2/1.08,0)</f>
-        <v>12593</v>
+        <f>ROUNDUP(B2*1.08,0)</f>
+        <v>14688</v>
       </c>
       <c r="C8" s="3">
-        <f>ROUNDUP(C2/1.08,0)</f>
-        <v>16667</v>
+        <f>ROUNDUP(C2*1.08,0)</f>
+        <v>19440</v>
       </c>
       <c r="D8" s="3">
-        <f>ROUNDUP(D2/1.08,0)</f>
-        <v>17593</v>
+        <f>ROUNDUP(D2*1.08,0)</f>
+        <v>20520</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1374,16 +1374,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <f>ROUNDUP(B3/1.08,0)</f>
-        <v>15186</v>
+        <f>ROUNDUP(B3*1.08,0)</f>
+        <v>17712</v>
       </c>
       <c r="C9" s="3">
-        <f>ROUNDUP(C3/1.08,0)</f>
-        <v>18519</v>
+        <f>ROUNDUP(C3*1.08,0)</f>
+        <v>21600</v>
       </c>
       <c r="D9" s="3">
-        <f>ROUNDUP(D3/1.08,0)</f>
-        <v>19445</v>
+        <f>ROUNDUP(D3*1.08,0)</f>
+        <v>22680</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1391,16 +1391,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <f>ROUNDUP(B4/1.08,0)</f>
-        <v>18519</v>
+        <f>ROUNDUP(B4*1.08,0)</f>
+        <v>21600</v>
       </c>
       <c r="C10" s="3">
-        <f>ROUNDUP(C4/1.08,0)</f>
-        <v>29075</v>
+        <f>ROUNDUP(C4*1.08,0)</f>
+        <v>33912</v>
       </c>
       <c r="D10" s="3">
-        <f>ROUNDUP(D4/1.08,0)</f>
-        <v>30556</v>
+        <f>ROUNDUP(D4*1.08,0)</f>
+        <v>35640</v>
       </c>
     </row>
     <row r="11" ht="29" spans="1:4">
@@ -1408,16 +1408,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <f>ROUNDUP(B5/1.08,0)</f>
-        <v>3704</v>
+        <f>ROUNDUP(B5*1.08,0)</f>
+        <v>4320</v>
       </c>
       <c r="C11" s="3">
-        <f>ROUNDUP(C5/1.08,0)</f>
-        <v>4445</v>
+        <f>ROUNDUP(C5*1.08,0)</f>
+        <v>5184</v>
       </c>
       <c r="D11" s="3">
-        <f>ROUNDUP(D5/1.08,0)</f>
-        <v>4630</v>
+        <f>ROUNDUP(D5*1.08,0)</f>
+        <v>5400</v>
       </c>
     </row>
   </sheetData>
@@ -1431,8 +1431,8 @@
   <sheetPr/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1588,24 +1588,24 @@
         <v>12</v>
       </c>
       <c r="B9" s="3">
-        <f>ROUNDUP(B2/1.08,0)</f>
-        <v>12593</v>
+        <f>ROUNDUP(B2*1.08,0)</f>
+        <v>14688</v>
       </c>
       <c r="C9" s="3">
-        <f>ROUNDUP(C2/1.08,0)</f>
-        <v>18056</v>
+        <f>ROUNDUP(C2*1.08,0)</f>
+        <v>21060</v>
       </c>
       <c r="D9" s="3">
-        <f>ROUNDUP(D2/1.08,0)</f>
-        <v>18982</v>
+        <f>ROUNDUP(D2*1.08,0)</f>
+        <v>22140</v>
       </c>
       <c r="E9" s="3">
-        <f>ROUNDUP(E2/1.08,0)</f>
-        <v>21297</v>
+        <f>ROUNDUP(E2*1.08,0)</f>
+        <v>24840</v>
       </c>
       <c r="F9" s="3">
-        <f>ROUNDUP(F2/1.08,0)</f>
-        <v>22686</v>
+        <f>ROUNDUP(F2*1.08,0)</f>
+        <v>26460</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1613,24 +1613,24 @@
         <v>13</v>
       </c>
       <c r="B10" s="3">
-        <f>ROUNDUP(B3/1.08,0)</f>
-        <v>15186</v>
+        <f>ROUNDUP(B3*1.08,0)</f>
+        <v>17712</v>
       </c>
       <c r="C10" s="3">
-        <f>ROUNDUP(C3/1.08,0)</f>
-        <v>24167</v>
+        <f>ROUNDUP(C3*1.08,0)</f>
+        <v>28188</v>
       </c>
       <c r="D10" s="3">
-        <f>ROUNDUP(D3/1.08,0)</f>
-        <v>25463</v>
+        <f>ROUNDUP(D3*1.08,0)</f>
+        <v>29700</v>
       </c>
       <c r="E10" s="3">
-        <f>ROUNDUP(E3/1.08,0)</f>
-        <v>28241</v>
+        <f>ROUNDUP(E3*1.08,0)</f>
+        <v>32940</v>
       </c>
       <c r="F10" s="3">
-        <f>ROUNDUP(F3/1.08,0)</f>
-        <v>30093</v>
+        <f>ROUNDUP(F3*1.08,0)</f>
+        <v>35100</v>
       </c>
     </row>
     <row r="11" ht="29" spans="1:6">
@@ -1638,24 +1638,24 @@
         <v>14</v>
       </c>
       <c r="B11" s="3">
-        <f>ROUNDUP(B4/1.08,0)</f>
-        <v>17686</v>
+        <f>ROUNDUP(B4*1.08,0)</f>
+        <v>20628</v>
       </c>
       <c r="C11" s="3">
-        <f>ROUNDUP(C4/1.08,0)</f>
-        <v>28612</v>
+        <f>ROUNDUP(C4*1.08,0)</f>
+        <v>33372</v>
       </c>
       <c r="D11" s="3">
-        <f>ROUNDUP(D4/1.08,0)</f>
-        <v>30093</v>
+        <f>ROUNDUP(D4*1.08,0)</f>
+        <v>35100</v>
       </c>
       <c r="E11" s="3">
-        <f>ROUNDUP(E4/1.08,0)</f>
-        <v>32871</v>
+        <f>ROUNDUP(E4*1.08,0)</f>
+        <v>38340</v>
       </c>
       <c r="F11" s="3">
-        <f>ROUNDUP(F4/1.08,0)</f>
-        <v>34723</v>
+        <f>ROUNDUP(F4*1.08,0)</f>
+        <v>40500</v>
       </c>
     </row>
     <row r="12" ht="29" spans="1:6">
@@ -1663,24 +1663,24 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <f>ROUNDUP(B5/1.08,0)</f>
-        <v>19352</v>
+        <f>ROUNDUP(B5*1.08,0)</f>
+        <v>22572</v>
       </c>
       <c r="C12" s="3">
-        <f>ROUNDUP(C5/1.08,0)</f>
-        <v>32038</v>
+        <f>ROUNDUP(C5*1.08,0)</f>
+        <v>37368</v>
       </c>
       <c r="D12" s="3">
-        <f>ROUNDUP(D5/1.08,0)</f>
-        <v>33797</v>
+        <f>ROUNDUP(D5*1.08,0)</f>
+        <v>39420</v>
       </c>
       <c r="E12" s="3">
-        <f>ROUNDUP(E5/1.08,0)</f>
-        <v>36575</v>
+        <f>ROUNDUP(E5*1.08,0)</f>
+        <v>42660</v>
       </c>
       <c r="F12" s="3">
-        <f>ROUNDUP(F5/1.08,0)</f>
-        <v>38426</v>
+        <f>ROUNDUP(F5*1.08,0)</f>
+        <v>44820</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1688,24 +1688,24 @@
         <v>16</v>
       </c>
       <c r="B13" s="3">
-        <f>ROUNDUP(B6/1.08,0)</f>
-        <v>2130</v>
+        <f>ROUNDUP(B6*1.08,0)</f>
+        <v>2484</v>
       </c>
       <c r="C13" s="3">
-        <f>ROUNDUP(C6/1.08,0)</f>
-        <v>2593</v>
+        <f>ROUNDUP(C6*1.08,0)</f>
+        <v>3024</v>
       </c>
       <c r="D13" s="3">
-        <f>ROUNDUP(D6/1.08,0)</f>
-        <v>2686</v>
+        <f>ROUNDUP(D6*1.08,0)</f>
+        <v>3132</v>
       </c>
       <c r="E13" s="3">
-        <f>ROUNDUP(E6/1.08,0)</f>
-        <v>3241</v>
+        <f>ROUNDUP(E6*1.08,0)</f>
+        <v>3780</v>
       </c>
       <c r="F13" s="3">
-        <f>ROUNDUP(F6/1.08,0)</f>
-        <v>3704</v>
+        <f>ROUNDUP(F6*1.08,0)</f>
+        <v>4320</v>
       </c>
     </row>
     <row r="15" spans="1:1">

</xml_diff>

<commit_message>
update hoàn chỉnh xuất báo giá PDF
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="19200" windowHeight="6920"/>
   </bookViews>
   <sheets>
-    <sheet name="Tiêu chuẩn TMĐT ĐG (CTN009)" sheetId="1" r:id="rId1"/>
+    <sheet name="Tiêu chuẩn TMĐT ĐG(CTN009)" sheetId="1" r:id="rId1"/>
     <sheet name="Tiêu chuẩn TMĐT(CTN007)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -31,7 +31,7 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>Nấc cước
-(Có VAT)</t>
+(Chưa VAT)</t>
   </si>
   <si>
     <t>Nội tỉnh cũ</t>
@@ -56,7 +56,7 @@
   </si>
   <si>
     <t>Nấc cước
-(Chưa VAT)</t>
+(Có VAT)</t>
   </si>
   <si>
     <t>Nội vùng</t>
@@ -1257,7 +1257,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="7" ht="29" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1445,7 +1445,7 @@
   <sheetData>
     <row r="1" ht="29" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="8" ht="29" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>

</xml_diff>